<commit_message>
answer Son's concern about LastLoggedTime when user change their system time
</commit_message>
<xml_diff>
--- a/01_DOCUMENT/Client Review.xlsx
+++ b/01_DOCUMENT/Client Review.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="165" yWindow="0" windowWidth="20610" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -289,6 +289,250 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Trong phần SMS List, thêm dòng thông báo số lượng SMS đã dùng ngay bên dưới Grid dữ liệu như sau.
+Used : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> SMS - Remaining : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> SMS.
+(You can send </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> SMS message per day)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Sơn] - Ok Đan. Sơn có chỉnh giao diện lại chút xíu.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Thêm chức năng View Info để khách hàng xem thông tin cơ bản của họ. (giống như bên Administrator)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Sơn] - Hiển thị thông tin ok rồi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>nhưng cần bung lớn bề rộng ra luôn, không cần hiển thị SMS List bên trái.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trong phần Customer, cho phép nhân viên Sales chỉnh sửa thêm mục CustomerType và Status.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Sơn] - Ok Đan.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trong phần Customer, thêm 1 text area để nhân viên Sales đó ghi chú thêm khi chỉnh sửa thông tin khách hàng.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Sơn] - Ok Đan.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trong phần View Log của Edited Customers, sau khi hoàn tất task thứ 5 thì ta có 2 grid dữ liệu :
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Customer Info </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(table Customers) và </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Edited Info </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(table CustomerLog)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Khi approve thì giữ nguyên và không delete record log đó đi trong table CustomerLog. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>---&gt; ok nhưng approve sai record</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+- Thêm 1 nút delete sau cột </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> để cho admin xóa sau. Click vào nút delete thì sẽ thực hiện xóa record log đó ra khỏi table CustomerLog. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">---&gt; cái này thì ok rồi Đan. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Khi xóa record cuối cùng thì grid hiển thị bị lỗi.</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">Hạn chế gửi tin nhắn trong 1 ngày của khách hàng, chỉ cho phép gửi 5 tin nhắn trong 1 ngày mà thôi. 
 Để làm được thì mình sẽ thêm 2 fields nữa vào table Customers trong Database là : LastLoggedDate và UsedSMS.
 Mỗi lần khách hàng reply lại sms thì mình sẽ kiểm tra 2 field này. Nếu đã gửi đủ 5 tin nhắn trong 1 ngày rồi thì Disable nút Reply (hiển thị nút Reply mờ) đi.
@@ -320,259 +564,25 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>[Sơn] - Có reset về 0 nhưng user có thể chỉnh lại ngày giờ trên máy là có thể gửi được nữa. Cho nên mình kiểm tra ngày trên database server chứ không phải ngày hệ thống.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Trong phần SMS List, thêm dòng thông báo số lượng SMS đã dùng ngay bên dưới Grid dữ liệu như sau.
-Used : </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> SMS - Remaining : </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> SMS.
-(You can send </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> SMS message per day)
+      <t xml:space="preserve">[Sơn] - Có reset về 0 nhưng user có thể chỉnh lại ngày giờ trên máy là có thể gửi được nữa. Cho nên mình kiểm tra ngày trên database server chứ không phải ngày hệ thống.
 </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[Sơn] - Ok Đan. Sơn có chỉnh giao diện lại chút xíu.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Thêm chức năng View Info để khách hàng xem thông tin cơ bản của họ. (giống như bên Administrator)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[Sơn] - Hiển thị thông tin ok rồi</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>nhưng cần bung lớn bề rộng ra luôn, không cần hiển thị SMS List bên trái.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Trong phần Customer, cho phép nhân viên Sales chỉnh sửa thêm mục CustomerType và Status.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[Sơn] - Ok Đan.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Trong phần Customer, thêm 1 text area để nhân viên Sales đó ghi chú thêm khi chỉnh sửa thông tin khách hàng.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[Sơn] - Ok Đan.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Trong phần View Log của Edited Customers, sau khi hoàn tất task thứ 5 thì ta có 2 grid dữ liệu :
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Customer Info </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(table Customers) và </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Edited Info </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(table CustomerLog)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">.
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Khi approve thì giữ nguyên và không delete record log đó đi trong table CustomerLog. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>---&gt; ok nhưng approve sai record</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-- Thêm 1 nút delete sau cột </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Status</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> để cho admin xóa sau. Click vào nút delete thì sẽ thực hiện xóa record log đó ra khỏi table CustomerLog. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">---&gt; cái này thì ok rồi Đan. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Khi xóa record cuối cùng thì grid hiển thị bị lỗi.</t>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Dan] LastLoggedDate la gio Server co`n khi user log vao system thi` minh lay gio Server de check chu ko lay gio client de check dau (server code ma`). Nen User co doi gio` cua ho cung ko anh huong dau Son, co the do Son test nen thay vay vi` may Son (client) cung la` server luon (co cai SQL Server)</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="13">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -650,6 +660,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000CC"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -881,7 +897,15 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FF0000CC"/>
+    </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1206,16 +1230,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14:XFD14"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.28515625" style="4" customWidth="1"/>
     <col min="2" max="2" width="108" style="1" bestFit="1" customWidth="1"/>
@@ -1225,7 +1249,7 @@
     <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
         <v>12</v>
       </c>
@@ -1233,13 +1257,13 @@
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1">
+    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1247,19 +1271,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="7" spans="1:9" s="9" customFormat="1" ht="21.95" customHeight="1">
+    <row r="7" spans="1:9" s="9" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
         <v>0</v>
       </c>
@@ -1274,7 +1298,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="3" customFormat="1" ht="45" customHeight="1">
+    <row r="8" spans="1:9" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="22">
         <v>1</v>
       </c>
@@ -1292,7 +1316,7 @@
       <c r="H8" s="28"/>
       <c r="I8" s="28"/>
     </row>
-    <row r="9" spans="1:9" s="3" customFormat="1" ht="45" customHeight="1">
+    <row r="9" spans="1:9" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="22">
         <v>2</v>
       </c>
@@ -1308,7 +1332,7 @@
       <c r="H9" s="28"/>
       <c r="I9" s="28"/>
     </row>
-    <row r="10" spans="1:9" s="3" customFormat="1" ht="45" customHeight="1">
+    <row r="10" spans="1:9" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="22">
         <v>3</v>
       </c>
@@ -1326,7 +1350,7 @@
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
     </row>
-    <row r="11" spans="1:9" s="3" customFormat="1" ht="45" customHeight="1">
+    <row r="11" spans="1:9" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="22">
         <v>4</v>
       </c>
@@ -1344,7 +1368,7 @@
       <c r="H11" s="28"/>
       <c r="I11" s="28"/>
     </row>
-    <row r="12" spans="1:9" s="3" customFormat="1" ht="45" customHeight="1">
+    <row r="12" spans="1:9" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="22">
         <v>5</v>
       </c>
@@ -1360,12 +1384,12 @@
       <c r="H12" s="28"/>
       <c r="I12" s="28"/>
     </row>
-    <row r="13" spans="1:9" s="3" customFormat="1" ht="75" customHeight="1">
+    <row r="13" spans="1:9" s="3" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="22">
         <v>6</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>14</v>
@@ -1376,12 +1400,12 @@
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
     </row>
-    <row r="14" spans="1:9" s="3" customFormat="1" ht="140.1" customHeight="1">
+    <row r="14" spans="1:9" s="3" customFormat="1" ht="140.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="22">
         <v>7</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="25"/>
@@ -1392,12 +1416,12 @@
       <c r="H14" s="28"/>
       <c r="I14" s="28"/>
     </row>
-    <row r="15" spans="1:9" s="3" customFormat="1" ht="80.099999999999994" customHeight="1">
+    <row r="15" spans="1:9" s="3" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22">
         <v>8</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="22"/>
       <c r="D15" s="25"/>
@@ -1408,12 +1432,12 @@
       <c r="H15" s="28"/>
       <c r="I15" s="28"/>
     </row>
-    <row r="16" spans="1:9" s="3" customFormat="1" ht="39.950000000000003" customHeight="1">
+    <row r="16" spans="1:9" s="3" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="22">
         <v>9</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="22"/>
       <c r="D16" s="25"/>
@@ -1424,12 +1448,12 @@
       <c r="H16" s="28"/>
       <c r="I16" s="28"/>
     </row>
-    <row r="17" spans="1:9" s="3" customFormat="1" ht="39.950000000000003" customHeight="1">
+    <row r="17" spans="1:9" s="3" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="22">
         <v>10</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="22"/>
       <c r="D17" s="24" t="s">
@@ -1440,12 +1464,12 @@
       <c r="H17" s="28"/>
       <c r="I17" s="28"/>
     </row>
-    <row r="18" spans="1:9" s="3" customFormat="1" ht="39.950000000000003" customHeight="1">
+    <row r="18" spans="1:9" s="3" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="22">
         <v>11</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="24" t="s">
         <v>14</v>
@@ -1458,14 +1482,14 @@
       <c r="H18" s="28"/>
       <c r="I18" s="28"/>
     </row>
-    <row r="19" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="19" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="10"/>
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
     </row>
-    <row r="20" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="20" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="18">
         <v>1</v>
       </c>
@@ -1483,7 +1507,7 @@
       <c r="H20" s="27"/>
       <c r="I20" s="27"/>
     </row>
-    <row r="21" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="21" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
         <v>2</v>
       </c>
@@ -1499,7 +1523,7 @@
       <c r="H21" s="27"/>
       <c r="I21" s="27"/>
     </row>
-    <row r="22" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="22" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
         <v>3</v>
       </c>
@@ -1515,7 +1539,7 @@
       <c r="H22" s="27"/>
       <c r="I22" s="27"/>
     </row>
-    <row r="23" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="23" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
         <v>4</v>
       </c>
@@ -1531,7 +1555,7 @@
       <c r="H23" s="27"/>
       <c r="I23" s="27"/>
     </row>
-    <row r="24" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="24" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="18">
         <v>5</v>
       </c>
@@ -1547,7 +1571,7 @@
       <c r="H24" s="27"/>
       <c r="I24" s="27"/>
     </row>
-    <row r="25" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="25" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18">
         <v>6</v>
       </c>
@@ -1563,140 +1587,140 @@
       <c r="H25" s="27"/>
       <c r="I25" s="27"/>
     </row>
-    <row r="26" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="26" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
       <c r="C26" s="10"/>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
     </row>
-    <row r="27" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="27" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
       <c r="B27" s="11"/>
       <c r="C27" s="10"/>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
     </row>
-    <row r="28" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="28" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10"/>
       <c r="B28" s="11"/>
       <c r="C28" s="10"/>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
     </row>
-    <row r="29" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="29" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10"/>
       <c r="B29" s="11"/>
       <c r="C29" s="10"/>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
     </row>
-    <row r="30" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="30" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="10"/>
       <c r="B30" s="11"/>
       <c r="C30" s="10"/>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
     </row>
-    <row r="31" spans="1:9" s="15" customFormat="1" ht="21.95" customHeight="1">
+    <row r="31" spans="1:9" s="15" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="13"/>
       <c r="B31" s="14"/>
       <c r="C31" s="13"/>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
     </row>
-    <row r="32" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="32" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="10"/>
       <c r="B32" s="11"/>
       <c r="C32" s="10"/>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
     </row>
-    <row r="33" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="33" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10"/>
       <c r="B33" s="11"/>
       <c r="C33" s="10"/>
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
     </row>
-    <row r="34" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="34" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="10"/>
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
     </row>
-    <row r="35" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="35" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="10"/>
       <c r="B35" s="11"/>
       <c r="C35" s="10"/>
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
     </row>
-    <row r="36" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="36" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10"/>
       <c r="B36" s="11"/>
       <c r="C36" s="10"/>
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
     </row>
-    <row r="37" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="37" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10"/>
       <c r="B37" s="11"/>
       <c r="C37" s="10"/>
       <c r="D37" s="12"/>
       <c r="E37" s="12"/>
     </row>
-    <row r="38" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="38" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10"/>
       <c r="B38" s="11"/>
       <c r="C38" s="10"/>
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
     </row>
-    <row r="39" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="39" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10"/>
       <c r="B39" s="11"/>
       <c r="C39" s="10"/>
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
     </row>
-    <row r="40" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="40" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10"/>
       <c r="B40" s="11"/>
       <c r="C40" s="10"/>
       <c r="D40" s="12"/>
       <c r="E40" s="12"/>
     </row>
-    <row r="41" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="41" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10"/>
       <c r="B41" s="11"/>
       <c r="C41" s="10"/>
       <c r="D41" s="12"/>
       <c r="E41" s="12"/>
     </row>
-    <row r="42" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="42" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="10"/>
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
     </row>
-    <row r="43" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="43" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="10"/>
       <c r="B43" s="11"/>
       <c r="C43" s="10"/>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
     </row>
-    <row r="44" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="44" spans="1:5" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10"/>
       <c r="B44" s="11"/>
       <c r="C44" s="10"/>
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
     </row>
-    <row r="45" spans="1:5" ht="21.95" customHeight="1">
+    <row r="45" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="16"/>
       <c r="B45" s="17"/>
       <c r="C45" s="16"/>
@@ -1718,12 +1742,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1732,12 +1756,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
update status of tasks
</commit_message>
<xml_diff>
--- a/01_DOCUMENT/Client Review.xlsx
+++ b/01_DOCUMENT/Client Review.xlsx
@@ -42,9 +42,6 @@
     <t>Trong phần Salesmen, khi thêm mới nhân viên Sales, cho mục chọn Group, Region, Area, Local</t>
   </si>
   <si>
-    <t>Trong phần Salesmen, thêm 2 combo box POC và POS để lọc dữ liệu</t>
-  </si>
-  <si>
     <t>Customer</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
   </si>
   <si>
     <t>þ</t>
-  </si>
-  <si>
-    <t>Trong phần Dashboard, thêm phần search và filter theo vùng (POC và POS).</t>
   </si>
   <si>
     <t>Phần màu vàng này Sơn sẽ giải thích thêm để Đan có thể hiểu được logic của nó. Mình sẽ voice trực tiếp qua skype nhé.
@@ -127,55 +121,6 @@
   </si>
   <si>
     <r>
-      <t>Trong phần Dashboard, thêm cột "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>view detail</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>" sau cột "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Content"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> để Administrator có thể xem thông tin chi tiết của dashboard giống như bên Salesmen.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[Sơn] - Hiện tại đã view được thông tin rồi nhưng giao diện chưa giồng với bên Salesmen. Đan chỉnh lại cho giống nhé.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Trong phần Dashboard, hiển thị mục </t>
     </r>
     <r>
@@ -208,72 +153,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Trong phần Customer, thêm chức năng lọc dữ liệu theo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>UPICode, Fullname</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> cho Grid dữ liệu </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Customer Management</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[Sơn] - Ok Đan. Cả 2 bên đều ok hết rồi.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Bên Administrator Đan cho thêm nút Clear giồng như bên Salesmen vô dùm Sơn nữa nhé. Thanks.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Trong phần View Log của Edited Customers, hiển thị thêm grid dữ liệu chưa chỉnh sửa (table Customers) của khách hàng đó để admin so sánh trước khi approve.
 </t>
     </r>
@@ -360,38 +239,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Thêm chức năng View Info để khách hàng xem thông tin cơ bản của họ. (giống như bên Administrator)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[Sơn] - Hiển thị thông tin ok rồi</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>nhưng cần bung lớn bề rộng ra luôn, không cần hiển thị SMS List bên trái.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Trong phần Customer, cho phép nhân viên Sales chỉnh sửa thêm mục CustomerType và Status.
 </t>
     </r>
@@ -418,117 +265,6 @@
         <family val="2"/>
       </rPr>
       <t>[Sơn] - Ok Đan.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Trong phần View Log của Edited Customers, sau khi hoàn tất task thứ 5 thì ta có 2 grid dữ liệu :
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Customer Info </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(table Customers) và </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Edited Info </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(table CustomerLog)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">.
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Khi approve thì giữ nguyên và không delete record log đó đi trong table CustomerLog. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>---&gt; ok nhưng approve sai record</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-- Thêm 1 nút delete sau cột </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Status</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> để cho admin xóa sau. Click vào nút delete thì sẽ thực hiện xóa record log đó ra khỏi table CustomerLog. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">---&gt; cái này thì ok rồi Đan. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Khi xóa record cuối cùng thì grid hiển thị bị lỗi.</t>
     </r>
   </si>
   <si>
@@ -575,6 +311,348 @@
         <family val="2"/>
       </rPr>
       <t>[Dan] LastLoggedDate la gio Server co`n khi user log vao system thi` minh lay gio Server de check chu ko lay gio client de check dau (server code ma`). Nen User co doi gio` cua ho cung ko anh huong dau Son, co the do Son test nen thay vay vi` may Son (client) cung la` server luon (co cai SQL Server)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trong phần Customer, thêm chức năng lọc dữ liệu theo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>UPICode, Fullname</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> cho Grid dữ liệu </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Customer Management</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Sơn] - Ok Đan. Cả 2 bên đều ok hết rồi.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Bên Administrator Đan cho thêm nút Clear giồng như bên Salesmen vô dùm Sơn nữa nhé. Thanks.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Dan] Done</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trong phần View Log của Edited Customers, sau khi hoàn tất task thứ 5 thì ta có 2 grid dữ liệu :
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Customer Info </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(table Customers) và </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Edited Info </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(table CustomerLog)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Khi approve thì giữ nguyên và không delete record log đó đi trong table CustomerLog. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">---&gt; ok nhưng approve sai record </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Dan] Fixed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+- Thêm 1 nút delete sau cột </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> để cho admin xóa sau. Click vào nút delete thì sẽ thực hiện xóa record log đó ra khỏi table CustomerLog. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">---&gt; cái này thì ok rồi Đan. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Khi xóa record cuối cùng thì grid hiển thị bị lỗi.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Dan] Fixed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Trong phần Dashboard, thêm cột "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>view detail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>" sau cột "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Content"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> để Administrator có thể xem thông tin chi tiết của dashboard giống như bên Salesmen.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Sơn] - Hiện tại đã view được thông tin rồi nhưng giao diện chưa giồng với bên Salesmen. Đan chỉnh lại cho giống nhé.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Dan] Giống như thế nào Sơn, mình thấy bên salesmen nó hiển thị details trên trang luôn chứ ko có popup, vậy là Son muốn hiển thị trên trang luôn phải không?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Thêm chức năng View Info để khách hàng xem thông tin cơ bản của họ. (giống như bên Administrator)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Sơn] - Hiển thị thông tin ok rồi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">nhưng cần bung lớn bề rộng ra luôn, không cần hiển thị SMS List bên trái. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Dan] Done</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trong phần Dashboard, thêm phần search và filter theo vùng (POC và POS).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Dan] Done</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trong phần Salesmen, thêm 2 combo box POC và POS để lọc dữ liệu
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Dan] Done</t>
     </r>
   </si>
 </sst>
@@ -582,7 +660,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -661,6 +739,13 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF0000CC"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color rgb="FF0000CC"/>
       <name val="Arial"/>
@@ -1234,9 +1319,9 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1251,7 +1336,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -1292,10 +1377,10 @@
         <v>5</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1303,15 +1388,15 @@
         <v>1</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="25"/>
       <c r="G8" s="28" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H8" s="28"/>
       <c r="I8" s="28"/>
@@ -1321,10 +1406,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="25"/>
@@ -1337,31 +1422,31 @@
         <v>3</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="25"/>
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
     </row>
-    <row r="11" spans="1:9" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" s="3" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="22">
         <v>4</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" s="25"/>
       <c r="G11" s="28"/>
@@ -1373,10 +1458,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
@@ -1389,10 +1474,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="25"/>
@@ -1405,12 +1490,12 @@
         <v>7</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="25"/>
       <c r="E14" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G14" s="28"/>
       <c r="H14" s="28"/>
@@ -1421,12 +1506,12 @@
         <v>8</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C15" s="22"/>
       <c r="D15" s="25"/>
       <c r="E15" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G15" s="28"/>
       <c r="H15" s="28"/>
@@ -1437,12 +1522,12 @@
         <v>9</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C16" s="22"/>
       <c r="D16" s="25"/>
       <c r="E16" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G16" s="28"/>
       <c r="H16" s="28"/>
@@ -1453,11 +1538,11 @@
         <v>10</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C17" s="22"/>
       <c r="D17" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E17" s="25"/>
       <c r="G17" s="28"/>
@@ -1469,13 +1554,13 @@
         <v>11</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E18" s="25"/>
       <c r="G18" s="28"/>
@@ -1494,15 +1579,15 @@
         <v>1</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="21"/>
       <c r="G20" s="26" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H20" s="27"/>
       <c r="I20" s="27"/>
@@ -1512,10 +1597,10 @@
         <v>2</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
@@ -1531,7 +1616,7 @@
         <v>6</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
@@ -1544,10 +1629,10 @@
         <v>4</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
@@ -1560,10 +1645,10 @@
         <v>5</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
@@ -1576,10 +1661,10 @@
         <v>6</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>

</xml_diff>

<commit_message>
update status of tasks - 2012-04-15
</commit_message>
<xml_diff>
--- a/01_DOCUMENT/Client Review.xlsx
+++ b/01_DOCUMENT/Client Review.xlsx
@@ -45,16 +45,10 @@
     <t>Trong phần Import Customer, chức năng import thực hiện sai.</t>
   </si>
   <si>
-    <t>Trong phần Phone List, hiển thị sai dữ liệu vì sai business rule. Filter để lọc bớt dữ liệu chứ không phải như hiện tại.</t>
-  </si>
-  <si>
     <t>Salesmen</t>
   </si>
   <si>
     <t>REVIEW SHEET</t>
-  </si>
-  <si>
-    <t>Trong phần Customer, thêm 1 cột hiển thị tên nhân viên Sales quản lý trực tiếp khách hàng đó.</t>
   </si>
   <si>
     <t>þ</t>
@@ -114,38 +108,6 @@
         <family val="2"/>
       </rPr>
       <t>[Sơn] - Ok Đan. Sơn có chỉnh giao diện lại chút xíu.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Trong phần Dashboard, hiển thị mục </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>download file</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (nếu có file đính kèm) khi xem thông tin chi tiết của dashboard.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[Sơn] - Bên Administrator thì ok rồi, còn bên Salesmen thì chưa có hiển thị.</t>
     </r>
   </si>
   <si>
@@ -666,6 +628,81 @@
         <family val="2"/>
       </rPr>
       <t>[Dan] Done</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trong phần Customer, thêm 1 cột hiển thị tên nhân viên Sales quản lý trực tiếp khách hàng đó.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Dan] Done</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trong phần Dashboard, hiển thị mục </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>download file</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (nếu có file đính kèm) khi xem thông tin chi tiết của dashboard.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Sơn] - Bên Administrator thì ok rồi, còn bên Salesmen thì chưa có hiển thị.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Dan] Co' roi ma` Son, check lai giup nhe</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trong phần Phone List, hiển thị sai dữ liệu vì sai business rule. Filter để lọc bớt dữ liệu chứ không phải như hiện tại.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Dan] Son noi ro giup minh Phone List nam o trang nao luon di, minh ko tim thay trong Administrator co cho na`o co Phone List het</t>
     </r>
   </si>
 </sst>
@@ -673,7 +710,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -761,6 +798,13 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF0000CC"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1332,9 +1376,9 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1349,7 +1393,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -1390,7 +1434,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>6</v>
@@ -1401,15 +1445,15 @@
         <v>1</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="25"/>
       <c r="G8" s="28" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H8" s="28"/>
       <c r="I8" s="28"/>
@@ -1419,10 +1463,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="25"/>
@@ -1435,13 +1479,13 @@
         <v>3</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E10" s="25"/>
       <c r="G10" s="28"/>
@@ -1453,13 +1497,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E11" s="25"/>
       <c r="G11" s="28"/>
@@ -1471,10 +1515,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
@@ -1487,10 +1531,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="25"/>
@@ -1498,17 +1542,17 @@
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
     </row>
-    <row r="14" spans="1:9" s="3" customFormat="1" ht="140.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" s="3" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
       <c r="A14" s="22">
         <v>7</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="25"/>
       <c r="E14" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G14" s="28"/>
       <c r="H14" s="28"/>
@@ -1519,12 +1563,12 @@
         <v>8</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C15" s="22"/>
       <c r="D15" s="25"/>
       <c r="E15" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G15" s="28"/>
       <c r="H15" s="28"/>
@@ -1535,12 +1579,12 @@
         <v>9</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C16" s="22"/>
       <c r="D16" s="25"/>
       <c r="E16" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G16" s="28"/>
       <c r="H16" s="28"/>
@@ -1551,11 +1595,11 @@
         <v>10</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C17" s="22"/>
       <c r="D17" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E17" s="25"/>
       <c r="G17" s="28"/>
@@ -1567,13 +1611,13 @@
         <v>11</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E18" s="25"/>
       <c r="G18" s="28"/>
@@ -1592,15 +1636,15 @@
         <v>1</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="21"/>
       <c r="G20" s="26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H20" s="27"/>
       <c r="I20" s="27"/>
@@ -1610,10 +1654,10 @@
         <v>2</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
@@ -1626,10 +1670,10 @@
         <v>3</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
@@ -1637,15 +1681,15 @@
       <c r="H22" s="27"/>
       <c r="I22" s="27"/>
     </row>
-    <row r="23" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
         <v>4</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
@@ -1653,15 +1697,15 @@
       <c r="H23" s="27"/>
       <c r="I23" s="27"/>
     </row>
-    <row r="24" spans="1:9" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" s="3" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="18">
         <v>5</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
@@ -1677,7 +1721,7 @@
         <v>7</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>

</xml_diff>

<commit_message>
Updateupdate status of tasks - 2012-04-17
</commit_message>
<xml_diff>
--- a/01_DOCUMENT/Client Review.xlsx
+++ b/01_DOCUMENT/Client Review.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="165" yWindow="0" windowWidth="20610" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Images" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$7:$F$25</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -313,6 +313,243 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Trong phần Customer, thêm chức năng lọc dữ liệu theo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>UPICode, Fullname</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> cho Grid dữ liệu </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Customer Management</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Sơn] - Ok Đan. Cả 2 bên đều ok hết rồi.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Bên Administrator Đan cho thêm nút Clear giồng như bên Salesmen vô dùm Sơn nữa nhé. Thanks.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Dan] Done
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Sơn] - Ok Đan.</t>
+    </r>
+  </si>
+  <si>
+    <t>% Status</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trong phần Dashboard, thêm phần search và filter theo vùng (POC và POS).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Dan] Done
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Sơn] - Khi filter thì dữ liệu ra chưa đúng. Sơn nghĩ là do import dữ liệu sai nên data bị sai. Cái này mình sẽ test lại sau khi làm xong chức năng import sau nha Đan.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trong phần Salesmen, thêm 2 combo box POC và POS để lọc dữ liệu
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Dan] Done
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Sơn] - Khi filter thì dữ liệu ra chưa đúng. Sơn nghĩ là do import dữ liệu sai nên data bị sai. Cái này mình sẽ test lại sau khi làm xong chức năng import sau nha Đan.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trong phần Import Customer, chức năng import thực hiện sai.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Dan] Son noi ro them la` sai nhu the nao voi nha, co`n file template de import la` file 20110516_Masterlist_Final.XLS (du`ng TAB [VmUpiDistributorCodes] phai ko Son? 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Sơn] - Đúng rồi Đan. Chức năng import hiện tại sai dữ liệu nên không thể hiện được mối quan hệ POC và POS, đồng thời khi mình search dữ liệu cũng ra sai thông tin luôn. Nên mình cần làm sạch lại database và sửa lại chức năng import để dữ liệu được import vào đúng table.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trong phần Dashboard, hiển thị mục </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>download file</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (nếu có file đính kèm) khi xem thông tin chi tiết của dashboard.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Sơn] - Bên Administrator thì ok rồi, còn bên Salesmen thì chưa có hiển thị.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Dan] Co' roi ma` Son, check lai giup nhe
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Sơn] - Bên ngoài grid Data thì có nhưng khi popup lên thì chưa có. Đan thử lại nhé.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Dan] Khi publish site se fix duoc cai Issue nay</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>Trong phần Dashboard, thêm cột "</t>
     </r>
     <r>
@@ -379,39 +616,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>[Sơn] - Sorry Đan, ý Sơn là giống như Dashboard của bên Sales Portal đó Đan. Đan login vào bên Sales Portal sẽ thấy.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Trong phần Dashboard, hiển thị mục </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>download file</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (nếu có file đính kèm) khi xem thông tin chi tiết của dashboard.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[Sơn] - Bên Administrator thì ok rồi, còn bên Salesmen thì chưa có hiển thị.
+      <t xml:space="preserve">[Sơn] - Sorry Đan, ý Sơn là giống như Dashboard của bên Sales Portal đó Đan. Đan login vào bên Sales Portal sẽ thấy.
 </t>
     </r>
     <r>
@@ -422,110 +627,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">[Dan] Co' roi ma` Son, check lai giup nhe
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[Sơn] - Bên ngoài grid Data thì có nhưng khi popup lên thì chưa có. Đan thử lại nhé.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Trong phần Customer, thêm chức năng lọc dữ liệu theo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>UPICode, Fullname</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> cho Grid dữ liệu </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Customer Management</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[Sơn] - Ok Đan. Cả 2 bên đều ok hết rồi.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Bên Administrator Đan cho thêm nút Clear giồng như bên Salesmen vô dùm Sơn nữa nhé. Thanks.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0000CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[Dan] Done
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[Sơn] - Ok Đan.</t>
-    </r>
-  </si>
-  <si>
-    <t>% Status</t>
+      <t>[Dan] Son coi lai coi duoc chua nha, thank you</t>
+    </r>
   </si>
   <si>
     <r>
@@ -665,12 +768,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Đan fix dùm Sơn bug khi xóa hết record rồi click nút Approve thì nó bị lỗi luôn nhé.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Trong phần Dashboard, thêm phần search và filter theo vùng (POC và POS).
+      <t xml:space="preserve">Đan fix dùm Sơn bug khi xóa hết record rồi click nút Approve thì nó bị lỗi luôn nhé.
 </t>
     </r>
     <r>
@@ -681,6 +779,22 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t>[Dan] fixed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trong phần Customer, thêm 1 cột hiển thị tên nhân viên Sales quản lý trực tiếp khách hàng đó.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">[Dan] Done
 </t>
     </r>
@@ -692,12 +806,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>[Sơn] - Khi filter thì dữ liệu ra chưa đúng. Sơn nghĩ là do import dữ liệu sai nên data bị sai. Cái này mình sẽ test lại sau khi làm xong chức năng import sau nha Đan.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Trong phần Salesmen, thêm 2 combo box POC và POS để lọc dữ liệu
+      <t xml:space="preserve">[Sơn] - Sơn không thấy.
 </t>
     </r>
     <r>
@@ -708,7 +817,23 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">[Dan] Done
+      <t>[Dan] Son coi hinh ben Sheet Images nha</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trong phần Salesmen, khi thêm mới nhân viên Sales, cho mục chọn Group, Region, Area, Local
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Dan] Done.
 </t>
     </r>
     <r>
@@ -719,12 +844,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>[Sơn] - Khi filter thì dữ liệu ra chưa đúng. Sơn nghĩ là do import dữ liệu sai nên data bị sai. Cái này mình sẽ test lại sau khi làm xong chức năng import sau nha Đan.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Trong phần Customer, thêm 1 cột hiển thị tên nhân viên Sales quản lý trực tiếp khách hàng đó.
+      <t xml:space="preserve">[Sơn] - Đan check lại giúp Sơn là chỉ có Rep mới chọn được Group, Region, Area, Local thôi nhé vì Rep là nhân viên sale quản lý trực tiếp khách hàng.
 </t>
     </r>
     <r>
@@ -735,7 +855,34 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">[Dan] Done
+      <t>[Dan] Done</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trong phần Phone List, hiển thị sai dữ liệu vì sai business rule. Filter để lọc bớt dữ liệu chứ không phải như hiện tại.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Dan] Son noi ro giup minh Phone List nam o trang nao luon di, minh ko tim thay trong Administrator co cho na`o co Phone List het
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Sơn] - Đan click vào SMS List &gt; Compose &gt; click nút Browse ở mục To... sẽ ra Phone List
 </t>
     </r>
     <r>
@@ -746,96 +893,15 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>[Sơn] - Sơn không thấy.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Trong phần Salesmen, khi thêm mới nhân viên Sales, cho mục chọn Group, Region, Area, Local
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0000CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[Dan] Done.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[Sơn] - Đan check lại giúp Sơn là chỉ có Rep mới chọn được Group, Region, Area, Local thôi nhé vì Rep là nhân viên sale quản lý trực tiếp khách hàng.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Trong phần Import Customer, chức năng import thực hiện sai.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[Dan] Son noi ro them la` sai nhu the nao voi nha, co`n file template de import la` file 20110516_Masterlist_Final.XLS (du`ng TAB [VmUpiDistributorCodes] phai ko Son? 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0000CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[Sơn] - Đúng rồi Đan. Chức năng import hiện tại sai dữ liệu nên không thể hiện được mối quan hệ POC và POS, đồng thời khi mình search dữ liệu cũng ra sai thông tin luôn. Nên mình cần làm sạch lại database và sửa lại chức năng import để dữ liệu được import vào đúng table.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Trong phần Phone List, hiển thị sai dữ liệu vì sai business rule. Filter để lọc bớt dữ liệu chứ không phải như hiện tại.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[Dan] Son noi ro giup minh Phone List nam o trang nao luon di, minh ko tim thay trong Administrator co cho na`o co Phone List het
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0000CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[Sơn] - Đan click vào SMS List &gt; Compose &gt; click nút Browse ở mục To... sẽ ra Phone List</t>
+      <t>[Dan] Done, co`n phan xoa cac Phone da gan thi` do cach lam hien tai hoi la. voi mi`nh nen chua co time coi, tam thoi de do di, chung nao co thoi gian minh se coi va lam them phan do</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="16">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1079,6 +1145,9 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1092,9 +1161,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1180,6 +1246,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10058400" cy="4693920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1503,17 +1618,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.28515625" style="4" customWidth="1"/>
     <col min="2" max="2" width="108" style="1" bestFit="1" customWidth="1"/>
@@ -1524,22 +1639,22 @@
     <col min="8" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="A1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-    </row>
-    <row r="2" spans="1:10" s="3" customFormat="1">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+    </row>
+    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="F2" s="32"/>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="F2" s="27"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1547,23 +1662,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="7" spans="1:10" s="9" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A7" s="30" t="s">
+    <row r="7" spans="1:10" s="9" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="30"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="8" t="s">
         <v>5</v>
       </c>
@@ -1574,10 +1689,10 @@
         <v>6</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="3" customFormat="1" ht="45" hidden="1" customHeight="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="3" customFormat="1" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="22">
         <v>1</v>
       </c>
@@ -1592,18 +1707,18 @@
       <c r="F8" s="22">
         <v>100</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="H8" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-    </row>
-    <row r="9" spans="1:10" s="3" customFormat="1" ht="84.75" customHeight="1">
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+    </row>
+    <row r="9" spans="1:10" s="3" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A9" s="22">
         <v>2</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C9" s="24" t="s">
         <v>9</v>
@@ -1611,16 +1726,16 @@
       <c r="D9" s="24"/>
       <c r="E9" s="25"/>
       <c r="F9" s="22"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-    </row>
-    <row r="10" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1">
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+    </row>
+    <row r="10" spans="1:10" s="3" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A10" s="22">
         <v>3</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C10" s="24" t="s">
         <v>9</v>
@@ -1630,16 +1745,16 @@
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="22"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-    </row>
-    <row r="11" spans="1:10" s="3" customFormat="1" ht="84.75" hidden="1" customHeight="1">
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+    </row>
+    <row r="11" spans="1:10" s="3" customFormat="1" ht="84.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="22">
         <v>4</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="24" t="s">
         <v>9</v>
@@ -1651,11 +1766,11 @@
       <c r="F11" s="22">
         <v>100</v>
       </c>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-    </row>
-    <row r="12" spans="1:10" s="3" customFormat="1" ht="54.75" hidden="1" customHeight="1">
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+    </row>
+    <row r="12" spans="1:10" s="3" customFormat="1" ht="54.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="22">
         <v>5</v>
       </c>
@@ -1670,16 +1785,16 @@
       <c r="F12" s="22">
         <v>100</v>
       </c>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-    </row>
-    <row r="13" spans="1:10" s="3" customFormat="1" ht="101.25" customHeight="1">
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+    </row>
+    <row r="13" spans="1:10" s="3" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="22">
         <v>6</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>9</v>
@@ -1689,11 +1804,11 @@
       <c r="F13" s="22">
         <v>98</v>
       </c>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-    </row>
-    <row r="14" spans="1:10" s="3" customFormat="1" ht="165.75" hidden="1">
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+    </row>
+    <row r="14" spans="1:10" s="3" customFormat="1" ht="165.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="22">
         <v>7</v>
       </c>
@@ -1708,11 +1823,11 @@
       <c r="F14" s="22">
         <v>100</v>
       </c>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-    </row>
-    <row r="15" spans="1:10" s="3" customFormat="1" ht="80.099999999999994" hidden="1" customHeight="1">
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+    </row>
+    <row r="15" spans="1:10" s="3" customFormat="1" ht="80.099999999999994" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22">
         <v>8</v>
       </c>
@@ -1727,11 +1842,11 @@
       <c r="F15" s="22">
         <v>100</v>
       </c>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-    </row>
-    <row r="16" spans="1:10" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1">
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+    </row>
+    <row r="16" spans="1:10" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="22">
         <v>9</v>
       </c>
@@ -1746,11 +1861,11 @@
       <c r="F16" s="22">
         <v>100</v>
       </c>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-    </row>
-    <row r="17" spans="1:10" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1">
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+    </row>
+    <row r="17" spans="1:10" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="22">
         <v>10</v>
       </c>
@@ -1765,11 +1880,11 @@
       <c r="F17" s="22">
         <v>100</v>
       </c>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-    </row>
-    <row r="18" spans="1:10" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1">
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+    </row>
+    <row r="18" spans="1:10" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="22">
         <v>11</v>
       </c>
@@ -1786,11 +1901,11 @@
       <c r="F18" s="22">
         <v>100</v>
       </c>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-    </row>
-    <row r="19" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1">
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+    </row>
+    <row r="19" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="10"/>
@@ -1798,12 +1913,12 @@
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
     </row>
-    <row r="20" spans="1:10" s="3" customFormat="1" ht="66" customHeight="1">
+    <row r="20" spans="1:10" s="3" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="18">
         <v>1</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>9</v>
@@ -1811,18 +1926,18 @@
       <c r="D20" s="21"/>
       <c r="E20" s="21"/>
       <c r="F20" s="18"/>
-      <c r="H20" s="27" t="s">
+      <c r="H20" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-    </row>
-    <row r="21" spans="1:10" s="3" customFormat="1" ht="66.75" customHeight="1">
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+    </row>
+    <row r="21" spans="1:10" s="3" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
         <v>2</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>9</v>
@@ -1830,16 +1945,16 @@
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
       <c r="F21" s="18"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-    </row>
-    <row r="22" spans="1:10" s="3" customFormat="1" ht="63.75" customHeight="1">
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+    </row>
+    <row r="22" spans="1:10" s="3" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
         <v>3</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>9</v>
@@ -1849,16 +1964,16 @@
       <c r="F22" s="18">
         <v>95</v>
       </c>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-    </row>
-    <row r="23" spans="1:10" s="3" customFormat="1" ht="50.1" customHeight="1">
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+    </row>
+    <row r="23" spans="1:10" s="3" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
         <v>4</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>9</v>
@@ -1866,11 +1981,11 @@
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
       <c r="F23" s="18"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-    </row>
-    <row r="24" spans="1:10" s="3" customFormat="1" ht="71.25" customHeight="1">
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+    </row>
+    <row r="24" spans="1:10" s="3" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="18">
         <v>5</v>
       </c>
@@ -1883,16 +1998,16 @@
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
       <c r="F24" s="18"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="28"/>
-    </row>
-    <row r="25" spans="1:10" s="3" customFormat="1" ht="99" customHeight="1">
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+    </row>
+    <row r="25" spans="1:10" s="3" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18">
         <v>6</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>9</v>
@@ -1900,11 +2015,11 @@
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
       <c r="F25" s="18"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-    </row>
-    <row r="26" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1">
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+    </row>
+    <row r="26" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
       <c r="C26" s="10"/>
@@ -1912,7 +2027,7 @@
       <c r="E26" s="12"/>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="27" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
       <c r="B27" s="11"/>
       <c r="C27" s="10"/>
@@ -1920,7 +2035,7 @@
       <c r="E27" s="12"/>
       <c r="F27" s="10"/>
     </row>
-    <row r="28" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="28" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10"/>
       <c r="B28" s="11"/>
       <c r="C28" s="10"/>
@@ -1928,7 +2043,7 @@
       <c r="E28" s="12"/>
       <c r="F28" s="10"/>
     </row>
-    <row r="29" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="29" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10"/>
       <c r="B29" s="11"/>
       <c r="C29" s="10"/>
@@ -1936,7 +2051,7 @@
       <c r="E29" s="12"/>
       <c r="F29" s="10"/>
     </row>
-    <row r="30" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="30" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="10"/>
       <c r="B30" s="11"/>
       <c r="C30" s="10"/>
@@ -1944,7 +2059,7 @@
       <c r="E30" s="12"/>
       <c r="F30" s="10"/>
     </row>
-    <row r="31" spans="1:10" s="15" customFormat="1" ht="21.95" customHeight="1">
+    <row r="31" spans="1:10" s="15" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="13"/>
       <c r="B31" s="14"/>
       <c r="C31" s="13"/>
@@ -1952,7 +2067,7 @@
       <c r="E31" s="14"/>
       <c r="F31" s="13"/>
     </row>
-    <row r="32" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="32" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="10"/>
       <c r="B32" s="11"/>
       <c r="C32" s="10"/>
@@ -1960,7 +2075,7 @@
       <c r="E32" s="12"/>
       <c r="F32" s="10"/>
     </row>
-    <row r="33" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="33" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10"/>
       <c r="B33" s="11"/>
       <c r="C33" s="10"/>
@@ -1968,7 +2083,7 @@
       <c r="E33" s="12"/>
       <c r="F33" s="10"/>
     </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="34" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="10"/>
@@ -1976,7 +2091,7 @@
       <c r="E34" s="12"/>
       <c r="F34" s="10"/>
     </row>
-    <row r="35" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="35" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="10"/>
       <c r="B35" s="11"/>
       <c r="C35" s="10"/>
@@ -1984,7 +2099,7 @@
       <c r="E35" s="12"/>
       <c r="F35" s="10"/>
     </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="36" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10"/>
       <c r="B36" s="11"/>
       <c r="C36" s="10"/>
@@ -1992,7 +2107,7 @@
       <c r="E36" s="12"/>
       <c r="F36" s="10"/>
     </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="37" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10"/>
       <c r="B37" s="11"/>
       <c r="C37" s="10"/>
@@ -2000,7 +2115,7 @@
       <c r="E37" s="12"/>
       <c r="F37" s="10"/>
     </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="38" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10"/>
       <c r="B38" s="11"/>
       <c r="C38" s="10"/>
@@ -2008,7 +2123,7 @@
       <c r="E38" s="12"/>
       <c r="F38" s="10"/>
     </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="39" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10"/>
       <c r="B39" s="11"/>
       <c r="C39" s="10"/>
@@ -2016,7 +2131,7 @@
       <c r="E39" s="12"/>
       <c r="F39" s="10"/>
     </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="40" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10"/>
       <c r="B40" s="11"/>
       <c r="C40" s="10"/>
@@ -2024,7 +2139,7 @@
       <c r="E40" s="12"/>
       <c r="F40" s="10"/>
     </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="41" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10"/>
       <c r="B41" s="11"/>
       <c r="C41" s="10"/>
@@ -2032,7 +2147,7 @@
       <c r="E41" s="12"/>
       <c r="F41" s="10"/>
     </row>
-    <row r="42" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="42" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="10"/>
@@ -2040,7 +2155,7 @@
       <c r="E42" s="12"/>
       <c r="F42" s="10"/>
     </row>
-    <row r="43" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="43" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="10"/>
       <c r="B43" s="11"/>
       <c r="C43" s="10"/>
@@ -2048,7 +2163,7 @@
       <c r="E43" s="12"/>
       <c r="F43" s="10"/>
     </row>
-    <row r="44" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="44" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10"/>
       <c r="B44" s="11"/>
       <c r="C44" s="10"/>
@@ -2056,7 +2171,7 @@
       <c r="E44" s="12"/>
       <c r="F44" s="10"/>
     </row>
-    <row r="45" spans="1:6" ht="21.95" customHeight="1">
+    <row r="45" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="16"/>
       <c r="B45" s="17"/>
       <c r="C45" s="16"/>
@@ -2068,7 +2183,7 @@
   <autoFilter ref="A7:F25">
     <filterColumn colId="0" showButton="0"/>
     <filterColumn colId="5">
-      <filters blank="1">
+      <filters>
         <filter val="98"/>
       </filters>
     </filterColumn>
@@ -2087,26 +2202,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
update status of tasks - 2012-04-20
</commit_message>
<xml_diff>
--- a/01_DOCUMENT/Client Review.xlsx
+++ b/01_DOCUMENT/Client Review.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="165" yWindow="0" windowWidth="20610" windowHeight="11640"/>
@@ -876,7 +876,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve"> 
+[Dan] Done, Son coi lai giup nhe</t>
     </r>
   </si>
   <si>
@@ -925,15 +926,26 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>[Sơn] - OK rồi Đan nhưng mình cần chỉnh sửa lại theo khái niệm POC và POS nữa thì mới đúng được. Để Sơn vẽ lại giao diện rồi mô tả thêm cho Đan dễ hiểu nha.</t>
+      <t xml:space="preserve">[Sơn] - OK rồi Đan nhưng mình cần chỉnh sửa lại theo khái niệm POC và POS nữa thì mới đúng được. Để Sơn vẽ lại giao diện rồi mô tả thêm cho Đan dễ hiểu nha.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Dan] Neu duoc Son cu mail cho tien nhe, vi gio giac hai ben chenh lech</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="16">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1306,7 +1318,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1650,17 +1662,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.28515625" style="4" customWidth="1"/>
     <col min="2" max="2" width="108" style="1" bestFit="1" customWidth="1"/>
@@ -1671,7 +1683,7 @@
     <col min="8" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30">
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
         <v>8</v>
       </c>
@@ -1679,14 +1691,14 @@
       <c r="C1" s="32"/>
       <c r="D1" s="32"/>
     </row>
-    <row r="2" spans="1:10" s="3" customFormat="1">
+    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="F2" s="27"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1694,19 +1706,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="7" spans="1:10" s="9" customFormat="1" ht="21.95" customHeight="1">
+    <row r="7" spans="1:10" s="9" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="31" t="s">
         <v>0</v>
       </c>
@@ -1724,7 +1736,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="3" customFormat="1" ht="45" hidden="1" customHeight="1">
+    <row r="8" spans="1:10" s="3" customFormat="1" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="22">
         <v>1</v>
       </c>
@@ -1745,7 +1757,7 @@
       <c r="I8" s="30"/>
       <c r="J8" s="30"/>
     </row>
-    <row r="9" spans="1:10" s="3" customFormat="1" ht="114.75">
+    <row r="9" spans="1:10" s="3" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A9" s="22">
         <v>2</v>
       </c>
@@ -1764,7 +1776,7 @@
       <c r="I9" s="30"/>
       <c r="J9" s="30"/>
     </row>
-    <row r="10" spans="1:10" s="3" customFormat="1" ht="80.25" hidden="1" customHeight="1">
+    <row r="10" spans="1:10" s="3" customFormat="1" ht="80.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="22">
         <v>3</v>
       </c>
@@ -1785,7 +1797,7 @@
       <c r="I10" s="30"/>
       <c r="J10" s="30"/>
     </row>
-    <row r="11" spans="1:10" s="3" customFormat="1" ht="84.75" hidden="1" customHeight="1">
+    <row r="11" spans="1:10" s="3" customFormat="1" ht="84.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="22">
         <v>4</v>
       </c>
@@ -1806,7 +1818,7 @@
       <c r="I11" s="30"/>
       <c r="J11" s="30"/>
     </row>
-    <row r="12" spans="1:10" s="3" customFormat="1" ht="54.75" hidden="1" customHeight="1">
+    <row r="12" spans="1:10" s="3" customFormat="1" ht="54.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="22">
         <v>5</v>
       </c>
@@ -1825,7 +1837,7 @@
       <c r="I12" s="30"/>
       <c r="J12" s="30"/>
     </row>
-    <row r="13" spans="1:10" s="3" customFormat="1" ht="101.25" hidden="1" customHeight="1">
+    <row r="13" spans="1:10" s="3" customFormat="1" ht="101.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="22">
         <v>6</v>
       </c>
@@ -1844,7 +1856,7 @@
       <c r="I13" s="30"/>
       <c r="J13" s="30"/>
     </row>
-    <row r="14" spans="1:10" s="3" customFormat="1" ht="165.75" hidden="1">
+    <row r="14" spans="1:10" s="3" customFormat="1" ht="165.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="22">
         <v>7</v>
       </c>
@@ -1863,7 +1875,7 @@
       <c r="I14" s="30"/>
       <c r="J14" s="30"/>
     </row>
-    <row r="15" spans="1:10" s="3" customFormat="1" ht="80.099999999999994" hidden="1" customHeight="1">
+    <row r="15" spans="1:10" s="3" customFormat="1" ht="80.099999999999994" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22">
         <v>8</v>
       </c>
@@ -1882,7 +1894,7 @@
       <c r="I15" s="30"/>
       <c r="J15" s="30"/>
     </row>
-    <row r="16" spans="1:10" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1">
+    <row r="16" spans="1:10" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="22">
         <v>9</v>
       </c>
@@ -1901,7 +1913,7 @@
       <c r="I16" s="30"/>
       <c r="J16" s="30"/>
     </row>
-    <row r="17" spans="1:10" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1">
+    <row r="17" spans="1:10" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="22">
         <v>10</v>
       </c>
@@ -1920,7 +1932,7 @@
       <c r="I17" s="30"/>
       <c r="J17" s="30"/>
     </row>
-    <row r="18" spans="1:10" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1">
+    <row r="18" spans="1:10" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="22">
         <v>11</v>
       </c>
@@ -1941,7 +1953,7 @@
       <c r="I18" s="30"/>
       <c r="J18" s="30"/>
     </row>
-    <row r="19" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="19" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="10"/>
@@ -1949,7 +1961,7 @@
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
     </row>
-    <row r="20" spans="1:10" s="3" customFormat="1" ht="66" customHeight="1">
+    <row r="20" spans="1:10" s="3" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="18">
         <v>1</v>
       </c>
@@ -1968,7 +1980,7 @@
       <c r="I20" s="29"/>
       <c r="J20" s="29"/>
     </row>
-    <row r="21" spans="1:10" s="3" customFormat="1" ht="66.75" customHeight="1">
+    <row r="21" spans="1:10" s="3" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
         <v>2</v>
       </c>
@@ -1985,7 +1997,7 @@
       <c r="I21" s="29"/>
       <c r="J21" s="29"/>
     </row>
-    <row r="22" spans="1:10" s="3" customFormat="1" ht="81.75" hidden="1" customHeight="1">
+    <row r="22" spans="1:10" s="3" customFormat="1" ht="81.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
         <v>3</v>
       </c>
@@ -2004,7 +2016,7 @@
       <c r="I22" s="29"/>
       <c r="J22" s="29"/>
     </row>
-    <row r="23" spans="1:10" s="3" customFormat="1" ht="69.75" hidden="1" customHeight="1">
+    <row r="23" spans="1:10" s="3" customFormat="1" ht="69.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
         <v>4</v>
       </c>
@@ -2023,7 +2035,7 @@
       <c r="I23" s="29"/>
       <c r="J23" s="29"/>
     </row>
-    <row r="24" spans="1:10" s="3" customFormat="1" ht="117.75" customHeight="1">
+    <row r="24" spans="1:10" s="3" customFormat="1" ht="117.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="18">
         <v>5</v>
       </c>
@@ -2040,7 +2052,7 @@
       <c r="I24" s="29"/>
       <c r="J24" s="29"/>
     </row>
-    <row r="25" spans="1:10" s="3" customFormat="1" ht="99" customHeight="1">
+    <row r="25" spans="1:10" s="3" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18">
         <v>6</v>
       </c>
@@ -2057,7 +2069,7 @@
       <c r="I25" s="29"/>
       <c r="J25" s="29"/>
     </row>
-    <row r="26" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="26" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
       <c r="C26" s="10"/>
@@ -2065,7 +2077,7 @@
       <c r="E26" s="12"/>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="27" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
       <c r="B27" s="11"/>
       <c r="C27" s="10"/>
@@ -2073,7 +2085,7 @@
       <c r="E27" s="12"/>
       <c r="F27" s="10"/>
     </row>
-    <row r="28" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="28" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10"/>
       <c r="B28" s="11"/>
       <c r="C28" s="10"/>
@@ -2081,7 +2093,7 @@
       <c r="E28" s="12"/>
       <c r="F28" s="10"/>
     </row>
-    <row r="29" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="29" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10"/>
       <c r="B29" s="11"/>
       <c r="C29" s="10"/>
@@ -2089,7 +2101,7 @@
       <c r="E29" s="12"/>
       <c r="F29" s="10"/>
     </row>
-    <row r="30" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="30" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="10"/>
       <c r="B30" s="11"/>
       <c r="C30" s="10"/>
@@ -2097,7 +2109,7 @@
       <c r="E30" s="12"/>
       <c r="F30" s="10"/>
     </row>
-    <row r="31" spans="1:10" s="15" customFormat="1" ht="21.95" customHeight="1">
+    <row r="31" spans="1:10" s="15" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="13"/>
       <c r="B31" s="14"/>
       <c r="C31" s="13"/>
@@ -2105,7 +2117,7 @@
       <c r="E31" s="14"/>
       <c r="F31" s="13"/>
     </row>
-    <row r="32" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="32" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="10"/>
       <c r="B32" s="11"/>
       <c r="C32" s="10"/>
@@ -2113,7 +2125,7 @@
       <c r="E32" s="12"/>
       <c r="F32" s="10"/>
     </row>
-    <row r="33" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="33" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10"/>
       <c r="B33" s="11"/>
       <c r="C33" s="10"/>
@@ -2121,7 +2133,7 @@
       <c r="E33" s="12"/>
       <c r="F33" s="10"/>
     </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="34" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="10"/>
@@ -2129,7 +2141,7 @@
       <c r="E34" s="12"/>
       <c r="F34" s="10"/>
     </row>
-    <row r="35" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="35" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="10"/>
       <c r="B35" s="11"/>
       <c r="C35" s="10"/>
@@ -2137,7 +2149,7 @@
       <c r="E35" s="12"/>
       <c r="F35" s="10"/>
     </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="36" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10"/>
       <c r="B36" s="11"/>
       <c r="C36" s="10"/>
@@ -2145,7 +2157,7 @@
       <c r="E36" s="12"/>
       <c r="F36" s="10"/>
     </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="37" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10"/>
       <c r="B37" s="11"/>
       <c r="C37" s="10"/>
@@ -2153,7 +2165,7 @@
       <c r="E37" s="12"/>
       <c r="F37" s="10"/>
     </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="38" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10"/>
       <c r="B38" s="11"/>
       <c r="C38" s="10"/>
@@ -2161,7 +2173,7 @@
       <c r="E38" s="12"/>
       <c r="F38" s="10"/>
     </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="39" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10"/>
       <c r="B39" s="11"/>
       <c r="C39" s="10"/>
@@ -2169,7 +2181,7 @@
       <c r="E39" s="12"/>
       <c r="F39" s="10"/>
     </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="40" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10"/>
       <c r="B40" s="11"/>
       <c r="C40" s="10"/>
@@ -2177,7 +2189,7 @@
       <c r="E40" s="12"/>
       <c r="F40" s="10"/>
     </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="41" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10"/>
       <c r="B41" s="11"/>
       <c r="C41" s="10"/>
@@ -2185,7 +2197,7 @@
       <c r="E41" s="12"/>
       <c r="F41" s="10"/>
     </row>
-    <row r="42" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="42" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="10"/>
@@ -2193,7 +2205,7 @@
       <c r="E42" s="12"/>
       <c r="F42" s="10"/>
     </row>
-    <row r="43" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="43" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="10"/>
       <c r="B43" s="11"/>
       <c r="C43" s="10"/>
@@ -2201,7 +2213,7 @@
       <c r="E43" s="12"/>
       <c r="F43" s="10"/>
     </row>
-    <row r="44" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="44" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10"/>
       <c r="B44" s="11"/>
       <c r="C44" s="10"/>
@@ -2209,7 +2221,7 @@
       <c r="E44" s="12"/>
       <c r="F44" s="10"/>
     </row>
-    <row r="45" spans="1:6" ht="21.95" customHeight="1">
+    <row r="45" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="16"/>
       <c r="B45" s="17"/>
       <c r="C45" s="16"/>
@@ -2221,7 +2233,7 @@
   <autoFilter ref="A7:F25">
     <filterColumn colId="0" showButton="0"/>
     <filterColumn colId="5">
-      <filters blank="1">
+      <filters>
         <filter val="90"/>
       </filters>
     </filterColumn>
@@ -2240,12 +2252,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2255,12 +2267,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add new field to client review to follow the "Need to review" status Add new SQL file to help create sample data
</commit_message>
<xml_diff>
--- a/01_DOCUMENT/Client Review.xlsx
+++ b/01_DOCUMENT/Client Review.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="165" yWindow="0" windowWidth="20610" windowHeight="11640"/>
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$7:$F$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$7:$G$25</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
   <si>
     <t>Task Name</t>
   </si>
@@ -1015,13 +1015,19 @@
       </rPr>
       <t xml:space="preserve"> này nhé.</t>
     </r>
+  </si>
+  <si>
+    <t>not yet</t>
+  </si>
+  <si>
+    <t>Need to review</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="16">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1119,8 +1125,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1163,6 +1175,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1191,7 +1209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1274,6 +1292,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1287,15 +1323,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1409,7 +1436,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1753,43 +1780,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.28515625" style="4" customWidth="1"/>
     <col min="2" max="2" width="108" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="4" customWidth="1"/>
-    <col min="4" max="5" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="2.28515625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="1"/>
+    <col min="4" max="6" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="2.28515625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A1" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-    </row>
-    <row r="2" spans="1:10" s="3" customFormat="1">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+    </row>
+    <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="F2" s="27"/>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="G2" s="27"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1797,23 +1824,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="7" spans="1:10" s="9" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A7" s="31" t="s">
+    <row r="7" spans="1:11" s="9" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="31"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="8" t="s">
         <v>5</v>
       </c>
@@ -1823,11 +1850,14 @@
       <c r="E7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="26" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="3" customFormat="1" ht="45" hidden="1" customHeight="1">
+    <row r="8" spans="1:11" s="3" customFormat="1" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="22">
         <v>1</v>
       </c>
@@ -1839,16 +1869,17 @@
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="25"/>
-      <c r="F8" s="22">
+      <c r="F8" s="25"/>
+      <c r="G8" s="22">
         <v>100</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="I8" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-    </row>
-    <row r="9" spans="1:10" s="3" customFormat="1" ht="127.5" hidden="1">
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+    </row>
+    <row r="9" spans="1:11" s="3" customFormat="1" ht="127.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="22">
         <v>2</v>
       </c>
@@ -1860,14 +1891,15 @@
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="25"/>
-      <c r="F9" s="22">
+      <c r="F9" s="25"/>
+      <c r="G9" s="22">
         <v>100</v>
       </c>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-    </row>
-    <row r="10" spans="1:10" s="3" customFormat="1" ht="80.25" hidden="1" customHeight="1">
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+    </row>
+    <row r="10" spans="1:11" s="3" customFormat="1" ht="80.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="22">
         <v>3</v>
       </c>
@@ -1881,14 +1913,15 @@
         <v>9</v>
       </c>
       <c r="E10" s="25"/>
-      <c r="F10" s="22">
+      <c r="F10" s="25"/>
+      <c r="G10" s="22">
         <v>100</v>
       </c>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-    </row>
-    <row r="11" spans="1:10" s="3" customFormat="1" ht="84.75" hidden="1" customHeight="1">
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+    </row>
+    <row r="11" spans="1:11" s="3" customFormat="1" ht="84.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="22">
         <v>4</v>
       </c>
@@ -1902,14 +1935,15 @@
         <v>9</v>
       </c>
       <c r="E11" s="25"/>
-      <c r="F11" s="22">
+      <c r="F11" s="25"/>
+      <c r="G11" s="22">
         <v>100</v>
       </c>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-    </row>
-    <row r="12" spans="1:10" s="3" customFormat="1" ht="54.75" hidden="1" customHeight="1">
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+    </row>
+    <row r="12" spans="1:11" s="3" customFormat="1" ht="54.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="22">
         <v>5</v>
       </c>
@@ -1921,14 +1955,15 @@
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
-      <c r="F12" s="22">
+      <c r="F12" s="25"/>
+      <c r="G12" s="22">
         <v>100</v>
       </c>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-    </row>
-    <row r="13" spans="1:10" s="3" customFormat="1" ht="133.5" customHeight="1">
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+    </row>
+    <row r="13" spans="1:11" s="3" customFormat="1" ht="133.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="22">
         <v>6</v>
       </c>
@@ -1940,14 +1975,17 @@
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="25"/>
-      <c r="F13" s="22">
+      <c r="F13" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="22">
         <v>95</v>
       </c>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-    </row>
-    <row r="14" spans="1:10" s="3" customFormat="1" ht="165.75" hidden="1">
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+    </row>
+    <row r="14" spans="1:11" s="3" customFormat="1" ht="165.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="22">
         <v>7</v>
       </c>
@@ -1959,14 +1997,15 @@
       <c r="E14" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="24"/>
+      <c r="G14" s="22">
         <v>100</v>
       </c>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-    </row>
-    <row r="15" spans="1:10" s="3" customFormat="1" ht="80.099999999999994" hidden="1" customHeight="1">
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+    </row>
+    <row r="15" spans="1:11" s="3" customFormat="1" ht="80.099999999999994" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22">
         <v>8</v>
       </c>
@@ -1978,14 +2017,15 @@
       <c r="E15" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="24"/>
+      <c r="G15" s="22">
         <v>100</v>
       </c>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-    </row>
-    <row r="16" spans="1:10" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1">
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="36"/>
+    </row>
+    <row r="16" spans="1:11" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="22">
         <v>9</v>
       </c>
@@ -1997,14 +2037,15 @@
       <c r="E16" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F16" s="24"/>
+      <c r="G16" s="22">
         <v>100</v>
       </c>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-    </row>
-    <row r="17" spans="1:10" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1">
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+    </row>
+    <row r="17" spans="1:11" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="22">
         <v>10</v>
       </c>
@@ -2016,14 +2057,15 @@
         <v>9</v>
       </c>
       <c r="E17" s="25"/>
-      <c r="F17" s="22">
+      <c r="F17" s="25"/>
+      <c r="G17" s="22">
         <v>100</v>
       </c>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-    </row>
-    <row r="18" spans="1:10" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1">
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+    </row>
+    <row r="18" spans="1:11" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="22">
         <v>11</v>
       </c>
@@ -2037,22 +2079,24 @@
         <v>9</v>
       </c>
       <c r="E18" s="25"/>
-      <c r="F18" s="22">
+      <c r="F18" s="25"/>
+      <c r="G18" s="22">
         <v>100</v>
       </c>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-    </row>
-    <row r="19" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1">
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+    </row>
+    <row r="19" spans="1:11" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="10"/>
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
-    </row>
-    <row r="20" spans="1:10" s="3" customFormat="1" ht="104.25" customHeight="1">
+      <c r="G19" s="12"/>
+    </row>
+    <row r="20" spans="1:11" s="3" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="18">
         <v>1</v>
       </c>
@@ -2064,16 +2108,19 @@
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="21"/>
-      <c r="F20" s="18">
+      <c r="F20" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="18">
         <v>10</v>
       </c>
-      <c r="H20" s="28" t="s">
+      <c r="I20" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-    </row>
-    <row r="21" spans="1:10" s="3" customFormat="1" ht="96" customHeight="1">
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
+    </row>
+    <row r="21" spans="1:11" s="3" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
         <v>2</v>
       </c>
@@ -2085,14 +2132,17 @@
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
-      <c r="F21" s="18">
+      <c r="F21" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="18">
         <v>80</v>
       </c>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-    </row>
-    <row r="22" spans="1:10" s="3" customFormat="1" ht="81.75" hidden="1" customHeight="1">
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
+    </row>
+    <row r="22" spans="1:11" s="3" customFormat="1" ht="81.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
         <v>3</v>
       </c>
@@ -2104,14 +2154,15 @@
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
-      <c r="F22" s="18">
+      <c r="F22" s="32"/>
+      <c r="G22" s="18">
         <v>100</v>
       </c>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-    </row>
-    <row r="23" spans="1:10" s="3" customFormat="1" ht="51" hidden="1">
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+    </row>
+    <row r="23" spans="1:11" s="3" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
         <v>4</v>
       </c>
@@ -2123,14 +2174,15 @@
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
-      <c r="F23" s="18">
+      <c r="F23" s="32"/>
+      <c r="G23" s="18">
         <v>100</v>
       </c>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-    </row>
-    <row r="24" spans="1:10" s="3" customFormat="1" ht="144" customHeight="1">
+      <c r="I23" s="35"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="35"/>
+    </row>
+    <row r="24" spans="1:11" s="3" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="18">
         <v>5</v>
       </c>
@@ -2142,12 +2194,15 @@
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
-      <c r="F24" s="18"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
-    </row>
-    <row r="25" spans="1:10" s="3" customFormat="1" ht="99" hidden="1" customHeight="1">
+      <c r="F24" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="18"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="35"/>
+    </row>
+    <row r="25" spans="1:11" s="3" customFormat="1" ht="99" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18">
         <v>6</v>
       </c>
@@ -2159,185 +2214,206 @@
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
-      <c r="F25" s="18">
+      <c r="F25" s="21"/>
+      <c r="G25" s="18">
         <v>100</v>
       </c>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
-    </row>
-    <row r="26" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1">
+      <c r="I25" s="35"/>
+      <c r="J25" s="35"/>
+      <c r="K25" s="35"/>
+    </row>
+    <row r="26" spans="1:11" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
       <c r="C26" s="10"/>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
-      <c r="F26" s="10"/>
-    </row>
-    <row r="27" spans="1:10" s="3" customFormat="1" ht="71.25" customHeight="1">
-      <c r="A27" s="33"/>
-      <c r="B27" s="34" t="s">
+      <c r="F26" s="12"/>
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" spans="1:11" s="3" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="29"/>
+      <c r="B27" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="35" t="s">
+      <c r="D27" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="35" t="s">
+      <c r="E27" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="33"/>
-    </row>
-    <row r="28" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1">
+      <c r="F27" s="31"/>
+      <c r="G27" s="29"/>
+    </row>
+    <row r="28" spans="1:11" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10"/>
       <c r="B28" s="11"/>
       <c r="C28" s="10"/>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
-      <c r="F28" s="10"/>
-    </row>
-    <row r="29" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1">
+      <c r="F28" s="12"/>
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" spans="1:11" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10"/>
       <c r="B29" s="11"/>
       <c r="C29" s="10"/>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
-      <c r="F29" s="10"/>
-    </row>
-    <row r="30" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1">
+      <c r="F29" s="12"/>
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" spans="1:11" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="10"/>
       <c r="B30" s="11"/>
       <c r="C30" s="10"/>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
-      <c r="F30" s="10"/>
-    </row>
-    <row r="31" spans="1:10" s="15" customFormat="1" ht="21.95" customHeight="1">
+      <c r="F30" s="12"/>
+      <c r="G30" s="10"/>
+    </row>
+    <row r="31" spans="1:11" s="15" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="13"/>
       <c r="B31" s="14"/>
       <c r="C31" s="13"/>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
-      <c r="F31" s="13"/>
-    </row>
-    <row r="32" spans="1:10" s="3" customFormat="1" ht="21.95" customHeight="1">
+      <c r="F31" s="14"/>
+      <c r="G31" s="13"/>
+    </row>
+    <row r="32" spans="1:11" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="10"/>
       <c r="B32" s="11"/>
       <c r="C32" s="10"/>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
-      <c r="F32" s="10"/>
-    </row>
-    <row r="33" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+      <c r="F32" s="12"/>
+      <c r="G32" s="10"/>
+    </row>
+    <row r="33" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10"/>
       <c r="B33" s="11"/>
       <c r="C33" s="10"/>
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
-      <c r="F33" s="10"/>
-    </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+      <c r="F33" s="12"/>
+      <c r="G33" s="10"/>
+    </row>
+    <row r="34" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="10"/>
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
-      <c r="F34" s="10"/>
-    </row>
-    <row r="35" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+      <c r="F34" s="12"/>
+      <c r="G34" s="10"/>
+    </row>
+    <row r="35" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="10"/>
       <c r="B35" s="11"/>
       <c r="C35" s="10"/>
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
-      <c r="F35" s="10"/>
-    </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+      <c r="F35" s="12"/>
+      <c r="G35" s="10"/>
+    </row>
+    <row r="36" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10"/>
       <c r="B36" s="11"/>
       <c r="C36" s="10"/>
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
-      <c r="F36" s="10"/>
-    </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+      <c r="F36" s="12"/>
+      <c r="G36" s="10"/>
+    </row>
+    <row r="37" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10"/>
       <c r="B37" s="11"/>
       <c r="C37" s="10"/>
       <c r="D37" s="12"/>
       <c r="E37" s="12"/>
-      <c r="F37" s="10"/>
-    </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+      <c r="F37" s="12"/>
+      <c r="G37" s="10"/>
+    </row>
+    <row r="38" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10"/>
       <c r="B38" s="11"/>
       <c r="C38" s="10"/>
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
-      <c r="F38" s="10"/>
-    </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+      <c r="F38" s="12"/>
+      <c r="G38" s="10"/>
+    </row>
+    <row r="39" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10"/>
       <c r="B39" s="11"/>
       <c r="C39" s="10"/>
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
-      <c r="F39" s="10"/>
-    </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+      <c r="F39" s="12"/>
+      <c r="G39" s="10"/>
+    </row>
+    <row r="40" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10"/>
       <c r="B40" s="11"/>
       <c r="C40" s="10"/>
       <c r="D40" s="12"/>
       <c r="E40" s="12"/>
-      <c r="F40" s="10"/>
-    </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+      <c r="F40" s="12"/>
+      <c r="G40" s="10"/>
+    </row>
+    <row r="41" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10"/>
       <c r="B41" s="11"/>
       <c r="C41" s="10"/>
       <c r="D41" s="12"/>
       <c r="E41" s="12"/>
-      <c r="F41" s="10"/>
-    </row>
-    <row r="42" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+      <c r="F41" s="12"/>
+      <c r="G41" s="10"/>
+    </row>
+    <row r="42" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="10"/>
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
-      <c r="F42" s="10"/>
-    </row>
-    <row r="43" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+      <c r="F42" s="12"/>
+      <c r="G42" s="10"/>
+    </row>
+    <row r="43" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="10"/>
       <c r="B43" s="11"/>
       <c r="C43" s="10"/>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
-      <c r="F43" s="10"/>
-    </row>
-    <row r="44" spans="1:6" s="3" customFormat="1" ht="21.95" customHeight="1">
+      <c r="F43" s="12"/>
+      <c r="G43" s="10"/>
+    </row>
+    <row r="44" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10"/>
       <c r="B44" s="11"/>
       <c r="C44" s="10"/>
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
-      <c r="F44" s="10"/>
-    </row>
-    <row r="45" spans="1:6" ht="21.95" customHeight="1">
+      <c r="F44" s="12"/>
+      <c r="G44" s="10"/>
+    </row>
+    <row r="45" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="16"/>
       <c r="B45" s="17"/>
       <c r="C45" s="16"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
-      <c r="F45" s="16"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="16"/>
     </row>
   </sheetData>
-  <autoFilter ref="A7:F25">
+  <autoFilter ref="A7:G25">
     <filterColumn colId="0" showButton="0"/>
-    <filterColumn colId="5">
+    <filterColumn colId="6">
       <filters blank="1">
         <filter val="10"/>
         <filter val="80"/>
@@ -2346,8 +2422,8 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="4">
-    <mergeCell ref="H20:J25"/>
-    <mergeCell ref="H8:J18"/>
+    <mergeCell ref="I20:K25"/>
+    <mergeCell ref="I8:K18"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A1:D1"/>
   </mergeCells>
@@ -2359,12 +2435,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2374,12 +2450,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix some minor issue
</commit_message>
<xml_diff>
--- a/01_DOCUMENT/Client Review.xlsx
+++ b/01_DOCUMENT/Client Review.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="165" yWindow="0" windowWidth="20610" windowHeight="11640"/>
@@ -708,6 +708,218 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Trong phần Phone List, hiển thị sai dữ liệu vì sai business rule. Filter để lọc bớt dữ liệu chứ không phải như hiện tại.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Dan] Son noi ro giup minh Phone List nam o trang nao luon di, minh ko tim thay trong Administrator co cho na`o co Phone List het
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Sơn] - Đan click vào SMS List &gt; Compose &gt; click nút Browse ở mục To... sẽ ra Phone List
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Dan] Done, co`n phan xoa cac Phone da gan thi` do cach lam hien tai hoi la. voi mi`nh nen chua co time coi, tam thoi de do di, chung nao co thoi gian minh se coi va lam them phan do
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Sơn] - OK rồi Đan nhưng mình cần chỉnh sửa lại theo khái niệm POC và POS nữa thì mới đúng được. Để Sơn vẽ lại giao diện rồi mô tả thêm cho Đan dễ hiểu nha.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Dan] Neu duoc Son cu mail cho tien nhe, vi gio giac hai ben chenh lech
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Dan] Son noi ro luon la` co can filter them theo POS POC cho phan nay ko nhe
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Sơn] - Cần Đan. Mình thêm POS POC cho cả 2 luôn nha (Salesmen và Customer). Thanks Đan.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trong phần Dashboard, thêm phần search và filter theo vùng (POC và POS).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Dan] Done
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Sơn] - Khi filter thì dữ liệu ra chưa đúng. Sơn nghĩ là do import dữ liệu sai nên data bị sai. Cái này mình sẽ test lại sau khi làm xong chức năng import sau nha Đan.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Sơn] - Khi chọn filter TROM thì TPS ra được danh sách, nhưng khi chọn TPS thì TPR không list ra được danh sách nhân viên Salesmen. Tương tự với PSR1 và PSR2 cũng không ra được danh sách nhân viên sales, Sơn xem bên phần Salesmen thì vẫn ra được kết quả.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Dan] da fixed. Son chu y la` phan Dashboard can phai co chua Phone Number dung voi du lieu import thi` Dashboard moi co du lieu nha
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Sơn] - Thanks Đan. Sơn sẽ test lại sau nhé.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trong phần Salesmen, thêm 2 combo box POC và POS để lọc dữ liệu
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Dan] Done
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Sơn] - Khi filter thì dữ liệu ra chưa đúng. Sơn nghĩ là do import dữ liệu sai nên data bị sai. Cái này mình sẽ test lại sau khi làm xong chức năng import sau nha Đan.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[Sơn] - Kết quả Filter và Search ra đúng rồi Đan. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Nhưng dữ liệu bị lặp lại khi mình filter theo Groups, Region, Area, Local nên mình cần Distince hoặc Group By lại sao cho mỗi tên Salesmen chỉ xuất hiện 1 lần trong grid Data mà thôi</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.
+[Dan] fixed
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Sơn] - Thanks Đan. Sơn sẽ test lại sau nhé.</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">Trong phần View Log của Edited Customers, sau khi hoàn tất task thứ 5 thì ta có 2 grid dữ liệu :
 - </t>
     </r>
@@ -888,227 +1100,17 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>[Sơn] - Vậy mình có thể cho dòng đó tô màu khác để đánh dấu là đã approve rồi được không Đan ?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Trong phần Phone List, hiển thị sai dữ liệu vì sai business rule. Filter để lọc bớt dữ liệu chứ không phải như hiện tại.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[Dan] Son noi ro giup minh Phone List nam o trang nao luon di, minh ko tim thay trong Administrator co cho na`o co Phone List het
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0000CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[Sơn] - Đan click vào SMS List &gt; Compose &gt; click nút Browse ở mục To... sẽ ra Phone List
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[Dan] Done, co`n phan xoa cac Phone da gan thi` do cach lam hien tai hoi la. voi mi`nh nen chua co time coi, tam thoi de do di, chung nao co thoi gian minh se coi va lam them phan do
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0000CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[Sơn] - OK rồi Đan nhưng mình cần chỉnh sửa lại theo khái niệm POC và POS nữa thì mới đúng được. Để Sơn vẽ lại giao diện rồi mô tả thêm cho Đan dễ hiểu nha.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[Dan] Neu duoc Son cu mail cho tien nhe, vi gio giac hai ben chenh lech
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0000CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[Dan] Son noi ro luon la` co can filter them theo POS POC cho phan nay ko nhe
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[Sơn] - Cần Đan. Mình thêm POS POC cho cả 2 luôn nha (Salesmen và Customer). Thanks Đan.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Trong phần Dashboard, thêm phần search và filter theo vùng (POC và POS).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0000CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[Dan] Done
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[Sơn] - Khi filter thì dữ liệu ra chưa đúng. Sơn nghĩ là do import dữ liệu sai nên data bị sai. Cái này mình sẽ test lại sau khi làm xong chức năng import sau nha Đan.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0000CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[Sơn] - Khi chọn filter TROM thì TPS ra được danh sách, nhưng khi chọn TPS thì TPR không list ra được danh sách nhân viên Salesmen. Tương tự với PSR1 và PSR2 cũng không ra được danh sách nhân viên sales, Sơn xem bên phần Salesmen thì vẫn ra được kết quả.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[Dan] da fixed. Son chu y la` phan Dashboard can phai co chua Phone Number dung voi du lieu import thi` Dashboard moi co du lieu nha
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0000CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[Sơn] - Thanks Đan. Sơn sẽ test lại sau nhé.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Trong phần Salesmen, thêm 2 combo box POC và POS để lọc dữ liệu
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0000CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[Dan] Done
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[Sơn] - Khi filter thì dữ liệu ra chưa đúng. Sơn nghĩ là do import dữ liệu sai nên data bị sai. Cái này mình sẽ test lại sau khi làm xong chức năng import sau nha Đan.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0000CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[Sơn] - Kết quả Filter và Search ra đúng rồi Đan. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Nhưng dữ liệu bị lặp lại khi mình filter theo Groups, Region, Area, Local nên mình cần Distince hoặc Group By lại sao cho mỗi tên Salesmen chỉ xuất hiện 1 lần trong grid Data mà thôi</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0000CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">.
-[Dan] fixed
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[Sơn] - Thanks Đan. Sơn sẽ test lại sau nhé.</t>
+      <t xml:space="preserve">[Sơn] - Vậy mình có thể cho dòng đó tô màu khác để đánh dấu là đã approve rồi được không Đan ?
+[Dan] Done
+</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="17">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1526,7 +1528,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1870,7 +1872,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K45"/>
   <sheetViews>
@@ -1880,7 +1882,7 @@
       <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.28515625" style="4" customWidth="1"/>
     <col min="2" max="2" width="108" style="1" bestFit="1" customWidth="1"/>
@@ -1891,7 +1893,7 @@
     <col min="9" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
         <v>8</v>
       </c>
@@ -1899,14 +1901,14 @@
       <c r="C1" s="39"/>
       <c r="D1" s="39"/>
     </row>
-    <row r="2" spans="1:11" s="3" customFormat="1">
+    <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="G2" s="27"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1914,19 +1916,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="7" spans="1:11" s="9" customFormat="1" ht="21.95" customHeight="1">
+    <row r="7" spans="1:11" s="9" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="38" t="s">
         <v>0</v>
       </c>
@@ -1947,7 +1949,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="3" customFormat="1" ht="45" hidden="1" customHeight="1">
+    <row r="8" spans="1:11" s="3" customFormat="1" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="22">
         <v>1</v>
       </c>
@@ -1969,7 +1971,7 @@
       <c r="J8" s="37"/>
       <c r="K8" s="37"/>
     </row>
-    <row r="9" spans="1:11" s="3" customFormat="1" ht="127.5" hidden="1">
+    <row r="9" spans="1:11" s="3" customFormat="1" ht="127.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="22">
         <v>2</v>
       </c>
@@ -1989,7 +1991,7 @@
       <c r="J9" s="37"/>
       <c r="K9" s="37"/>
     </row>
-    <row r="10" spans="1:11" s="3" customFormat="1" ht="80.25" hidden="1" customHeight="1">
+    <row r="10" spans="1:11" s="3" customFormat="1" ht="80.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="22">
         <v>3</v>
       </c>
@@ -2011,7 +2013,7 @@
       <c r="J10" s="37"/>
       <c r="K10" s="37"/>
     </row>
-    <row r="11" spans="1:11" s="3" customFormat="1" ht="84.75" hidden="1" customHeight="1">
+    <row r="11" spans="1:11" s="3" customFormat="1" ht="84.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="22">
         <v>4</v>
       </c>
@@ -2033,7 +2035,7 @@
       <c r="J11" s="37"/>
       <c r="K11" s="37"/>
     </row>
-    <row r="12" spans="1:11" s="3" customFormat="1" ht="54.75" hidden="1" customHeight="1">
+    <row r="12" spans="1:11" s="3" customFormat="1" ht="54.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="22">
         <v>5</v>
       </c>
@@ -2053,20 +2055,20 @@
       <c r="J12" s="37"/>
       <c r="K12" s="37"/>
     </row>
-    <row r="13" spans="1:11" s="3" customFormat="1" ht="195.75" customHeight="1">
+    <row r="13" spans="1:11" s="3" customFormat="1" ht="195.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="22">
         <v>6</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="25"/>
-      <c r="F13" s="33" t="s">
-        <v>28</v>
+      <c r="F13" s="34" t="s">
+        <v>29</v>
       </c>
       <c r="G13" s="22">
         <v>95</v>
@@ -2075,7 +2077,7 @@
       <c r="J13" s="37"/>
       <c r="K13" s="37"/>
     </row>
-    <row r="14" spans="1:11" s="3" customFormat="1" ht="165.75" hidden="1">
+    <row r="14" spans="1:11" s="3" customFormat="1" ht="165.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="22">
         <v>7</v>
       </c>
@@ -2095,7 +2097,7 @@
       <c r="J14" s="37"/>
       <c r="K14" s="37"/>
     </row>
-    <row r="15" spans="1:11" s="3" customFormat="1" ht="80.099999999999994" hidden="1" customHeight="1">
+    <row r="15" spans="1:11" s="3" customFormat="1" ht="80.099999999999994" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22">
         <v>8</v>
       </c>
@@ -2115,7 +2117,7 @@
       <c r="J15" s="37"/>
       <c r="K15" s="37"/>
     </row>
-    <row r="16" spans="1:11" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1">
+    <row r="16" spans="1:11" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="22">
         <v>9</v>
       </c>
@@ -2135,7 +2137,7 @@
       <c r="J16" s="37"/>
       <c r="K16" s="37"/>
     </row>
-    <row r="17" spans="1:11" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1">
+    <row r="17" spans="1:11" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="22">
         <v>10</v>
       </c>
@@ -2155,7 +2157,7 @@
       <c r="J17" s="37"/>
       <c r="K17" s="37"/>
     </row>
-    <row r="18" spans="1:11" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1">
+    <row r="18" spans="1:11" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="22">
         <v>11</v>
       </c>
@@ -2177,7 +2179,7 @@
       <c r="J18" s="37"/>
       <c r="K18" s="37"/>
     </row>
-    <row r="19" spans="1:11" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="19" spans="1:11" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="10"/>
@@ -2186,12 +2188,12 @@
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
     </row>
-    <row r="20" spans="1:11" s="3" customFormat="1" ht="143.25" customHeight="1">
+    <row r="20" spans="1:11" s="3" customFormat="1" ht="143.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="18">
         <v>1</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>9</v>
@@ -2210,12 +2212,12 @@
       <c r="J20" s="36"/>
       <c r="K20" s="36"/>
     </row>
-    <row r="21" spans="1:11" s="3" customFormat="1" ht="116.25" customHeight="1">
+    <row r="21" spans="1:11" s="3" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
         <v>2</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>9</v>
@@ -2232,7 +2234,7 @@
       <c r="J21" s="36"/>
       <c r="K21" s="36"/>
     </row>
-    <row r="22" spans="1:11" s="3" customFormat="1" ht="81.75" hidden="1" customHeight="1">
+    <row r="22" spans="1:11" s="3" customFormat="1" ht="81.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
         <v>3</v>
       </c>
@@ -2252,7 +2254,7 @@
       <c r="J22" s="36"/>
       <c r="K22" s="36"/>
     </row>
-    <row r="23" spans="1:11" s="3" customFormat="1" ht="51" hidden="1">
+    <row r="23" spans="1:11" s="3" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
         <v>4</v>
       </c>
@@ -2272,12 +2274,12 @@
       <c r="J23" s="36"/>
       <c r="K23" s="36"/>
     </row>
-    <row r="24" spans="1:11" s="3" customFormat="1" ht="153" customHeight="1">
+    <row r="24" spans="1:11" s="3" customFormat="1" ht="153" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="18">
         <v>5</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="20" t="s">
         <v>9</v>
@@ -2292,7 +2294,7 @@
       <c r="J24" s="36"/>
       <c r="K24" s="36"/>
     </row>
-    <row r="25" spans="1:11" s="3" customFormat="1" ht="99" hidden="1" customHeight="1">
+    <row r="25" spans="1:11" s="3" customFormat="1" ht="99" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18">
         <v>6</v>
       </c>
@@ -2312,7 +2314,7 @@
       <c r="J25" s="36"/>
       <c r="K25" s="36"/>
     </row>
-    <row r="26" spans="1:11" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="26" spans="1:11" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
       <c r="C26" s="10"/>
@@ -2321,7 +2323,7 @@
       <c r="F26" s="12"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:11" s="3" customFormat="1" ht="71.25" customHeight="1">
+    <row r="27" spans="1:11" s="3" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="29"/>
       <c r="B27" s="30" t="s">
         <v>26</v>
@@ -2338,7 +2340,7 @@
       <c r="F27" s="31"/>
       <c r="G27" s="29"/>
     </row>
-    <row r="28" spans="1:11" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="28" spans="1:11" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10"/>
       <c r="B28" s="11"/>
       <c r="C28" s="10"/>
@@ -2347,7 +2349,7 @@
       <c r="F28" s="12"/>
       <c r="G28" s="10"/>
     </row>
-    <row r="29" spans="1:11" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="29" spans="1:11" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10"/>
       <c r="B29" s="11"/>
       <c r="C29" s="10"/>
@@ -2356,7 +2358,7 @@
       <c r="F29" s="12"/>
       <c r="G29" s="10"/>
     </row>
-    <row r="30" spans="1:11" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="30" spans="1:11" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="10"/>
       <c r="B30" s="11"/>
       <c r="C30" s="10"/>
@@ -2365,7 +2367,7 @@
       <c r="F30" s="12"/>
       <c r="G30" s="10"/>
     </row>
-    <row r="31" spans="1:11" s="15" customFormat="1" ht="21.95" customHeight="1">
+    <row r="31" spans="1:11" s="15" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="13"/>
       <c r="B31" s="14"/>
       <c r="C31" s="13"/>
@@ -2374,7 +2376,7 @@
       <c r="F31" s="14"/>
       <c r="G31" s="13"/>
     </row>
-    <row r="32" spans="1:11" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="32" spans="1:11" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="10"/>
       <c r="B32" s="11"/>
       <c r="C32" s="10"/>
@@ -2383,7 +2385,7 @@
       <c r="F32" s="12"/>
       <c r="G32" s="10"/>
     </row>
-    <row r="33" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="33" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10"/>
       <c r="B33" s="11"/>
       <c r="C33" s="10"/>
@@ -2392,7 +2394,7 @@
       <c r="F33" s="12"/>
       <c r="G33" s="10"/>
     </row>
-    <row r="34" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="34" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="10"/>
@@ -2401,7 +2403,7 @@
       <c r="F34" s="12"/>
       <c r="G34" s="10"/>
     </row>
-    <row r="35" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="35" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="10"/>
       <c r="B35" s="11"/>
       <c r="C35" s="10"/>
@@ -2410,7 +2412,7 @@
       <c r="F35" s="12"/>
       <c r="G35" s="10"/>
     </row>
-    <row r="36" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="36" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10"/>
       <c r="B36" s="11"/>
       <c r="C36" s="10"/>
@@ -2419,7 +2421,7 @@
       <c r="F36" s="12"/>
       <c r="G36" s="10"/>
     </row>
-    <row r="37" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="37" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10"/>
       <c r="B37" s="11"/>
       <c r="C37" s="10"/>
@@ -2428,7 +2430,7 @@
       <c r="F37" s="12"/>
       <c r="G37" s="10"/>
     </row>
-    <row r="38" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="38" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10"/>
       <c r="B38" s="11"/>
       <c r="C38" s="10"/>
@@ -2437,7 +2439,7 @@
       <c r="F38" s="12"/>
       <c r="G38" s="10"/>
     </row>
-    <row r="39" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="39" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10"/>
       <c r="B39" s="11"/>
       <c r="C39" s="10"/>
@@ -2446,7 +2448,7 @@
       <c r="F39" s="12"/>
       <c r="G39" s="10"/>
     </row>
-    <row r="40" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="40" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10"/>
       <c r="B40" s="11"/>
       <c r="C40" s="10"/>
@@ -2455,7 +2457,7 @@
       <c r="F40" s="12"/>
       <c r="G40" s="10"/>
     </row>
-    <row r="41" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="41" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10"/>
       <c r="B41" s="11"/>
       <c r="C41" s="10"/>
@@ -2464,7 +2466,7 @@
       <c r="F41" s="12"/>
       <c r="G41" s="10"/>
     </row>
-    <row r="42" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="42" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="10"/>
@@ -2473,7 +2475,7 @@
       <c r="F42" s="12"/>
       <c r="G42" s="10"/>
     </row>
-    <row r="43" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="43" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="10"/>
       <c r="B43" s="11"/>
       <c r="C43" s="10"/>
@@ -2482,7 +2484,7 @@
       <c r="F43" s="12"/>
       <c r="G43" s="10"/>
     </row>
-    <row r="44" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1">
+    <row r="44" spans="1:7" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10"/>
       <c r="B44" s="11"/>
       <c r="C44" s="10"/>
@@ -2491,7 +2493,7 @@
       <c r="F44" s="12"/>
       <c r="G44" s="10"/>
     </row>
-    <row r="45" spans="1:7" ht="21.95" customHeight="1">
+    <row r="45" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="16"/>
       <c r="B45" s="17"/>
       <c r="C45" s="16"/>
@@ -2525,12 +2527,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2540,12 +2542,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
SQL script for Promotion Search History update Client Review file
</commit_message>
<xml_diff>
--- a/01_DOCUMENT/Client Review.xlsx
+++ b/01_DOCUMENT/Client Review.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="60" windowWidth="20610" windowHeight="11580"/>
+    <workbookView xWindow="165" yWindow="60" windowWidth="19320" windowHeight="11580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1509,6 +1509,9 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1523,9 +1526,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2059,7 +2059,7 @@
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
-      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2074,12 +2074,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
@@ -2110,10 +2110,10 @@
       <c r="D5" s="7"/>
     </row>
     <row r="7" spans="1:11" s="9" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="41"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="8" t="s">
         <v>5</v>
       </c>
@@ -2146,11 +2146,11 @@
       <c r="G8" s="20">
         <v>100</v>
       </c>
-      <c r="I8" s="40" t="s">
+      <c r="I8" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="40"/>
-      <c r="K8" s="40"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
     </row>
     <row r="9" spans="1:11" s="3" customFormat="1" ht="127.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="20">
@@ -2168,9 +2168,9 @@
       <c r="G9" s="20">
         <v>100</v>
       </c>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="80.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="20">
@@ -2190,9 +2190,9 @@
       <c r="G10" s="20">
         <v>100</v>
       </c>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
     </row>
     <row r="11" spans="1:11" s="3" customFormat="1" ht="84.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20">
@@ -2212,9 +2212,9 @@
       <c r="G11" s="20">
         <v>100</v>
       </c>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
     </row>
     <row r="12" spans="1:11" s="3" customFormat="1" ht="54.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="20">
@@ -2232,9 +2232,9 @@
       <c r="G12" s="20">
         <v>100</v>
       </c>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="40"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="41"/>
     </row>
     <row r="13" spans="1:11" s="3" customFormat="1" ht="195.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="20">
@@ -2254,9 +2254,9 @@
       <c r="G13" s="20">
         <v>100</v>
       </c>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="40"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
     </row>
     <row r="14" spans="1:11" s="3" customFormat="1" ht="165.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="20">
@@ -2274,9 +2274,9 @@
       <c r="G14" s="20">
         <v>100</v>
       </c>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="40"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
     </row>
     <row r="15" spans="1:11" s="3" customFormat="1" ht="80.099999999999994" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="20">
@@ -2294,9 +2294,9 @@
       <c r="G15" s="20">
         <v>100</v>
       </c>
-      <c r="I15" s="40"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="40"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41"/>
     </row>
     <row r="16" spans="1:11" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20">
@@ -2314,9 +2314,9 @@
       <c r="G16" s="20">
         <v>100</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="40"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="41"/>
     </row>
     <row r="17" spans="1:11" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20">
@@ -2334,9 +2334,9 @@
       <c r="G17" s="20">
         <v>100</v>
       </c>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="40"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="41"/>
     </row>
     <row r="18" spans="1:11" s="3" customFormat="1" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20">
@@ -2356,9 +2356,9 @@
       <c r="G18" s="20">
         <v>100</v>
       </c>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="41"/>
     </row>
     <row r="19" spans="1:11" s="3" customFormat="1" ht="143.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="16">
@@ -2378,11 +2378,11 @@
       <c r="G19" s="16">
         <v>100</v>
       </c>
-      <c r="I19" s="38" t="s">
+      <c r="I19" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="J19" s="39"/>
-      <c r="K19" s="39"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
     </row>
     <row r="20" spans="1:11" s="3" customFormat="1" ht="116.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="16">
@@ -2402,9 +2402,9 @@
       <c r="G20" s="16">
         <v>100</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="39"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
     </row>
     <row r="21" spans="1:11" s="3" customFormat="1" ht="81.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="16">
@@ -2422,9 +2422,9 @@
       <c r="G21" s="16">
         <v>100</v>
       </c>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
     </row>
     <row r="22" spans="1:11" s="3" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="16">
@@ -2442,9 +2442,9 @@
       <c r="G22" s="16">
         <v>100</v>
       </c>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="40"/>
     </row>
     <row r="23" spans="1:11" s="3" customFormat="1" ht="165.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="16">
@@ -2464,9 +2464,9 @@
       <c r="G23" s="16">
         <v>100</v>
       </c>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
     </row>
     <row r="24" spans="1:11" s="3" customFormat="1" ht="99" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="16">
@@ -2484,9 +2484,9 @@
       <c r="G24" s="16">
         <v>100</v>
       </c>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
     </row>
     <row r="25" spans="1:11" s="3" customFormat="1" ht="71.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="26"/>
@@ -2520,8 +2520,8 @@
       <c r="D26" s="32"/>
       <c r="E26" s="32"/>
       <c r="F26" s="33"/>
-      <c r="G26" s="10">
-        <v>0</v>
+      <c r="G26" s="37">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="13" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2538,7 +2538,7 @@
       <c r="G27" s="37">
         <v>1</v>
       </c>
-      <c r="I27" s="43" t="s">
+      <c r="I27" s="38" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2752,7 +2752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="S7:S64"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="S69" sqref="S69"/>
     </sheetView>
   </sheetViews>

</xml_diff>